<commit_message>
przeście na sterowanie z przeglądarki
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n.sarapata\Desktop\CreativeCreator - LinkTXT - automatyczny\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n.sarapata\Desktop\CreativeCreator - LinkTXT - automatyczny — kopia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD4FF9D-E408-457B-BC51-F77DD01913FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24205876-13E8-4A03-976B-E937C397BC2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-49200" yWindow="-15375" windowWidth="25095" windowHeight="20505" xr2:uid="{268508D8-A5A5-43C6-B277-EABFD88C5871}"/>
+    <workbookView xWindow="-49680" yWindow="-15375" windowWidth="25095" windowHeight="20505" xr2:uid="{268508D8-A5A5-43C6-B277-EABFD88C5871}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -404,7 +404,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -433,7 +433,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>93931</v>
+        <v>88278</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>

</xml_diff>